<commit_message>
oh no big problems
Also got the dijOnly graphs
</commit_message>
<xml_diff>
--- a/graphs long term.xlsx
+++ b/graphs long term.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjmd1g17\Documents\Fair-Vehicle-Routing-Simple-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C5DE8A-30BA-491E-BD1F-C380DA148645}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7748A1C4-3237-4BCB-911A-937BDE92EEAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" tabRatio="872" activeTab="1" xr2:uid="{7A734B0F-1E96-45C2-88D2-05431AC6EABE}"/>
   </bookViews>
@@ -24768,11 +24768,11 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <f>H2/D2</f>
+        <f t="shared" ref="J2:J9" si="0">H2/D2</f>
         <v>1</v>
       </c>
       <c r="K2">
-        <f>I2/D2</f>
+        <f t="shared" ref="K2:K9" si="1">I2/D2</f>
         <v>1</v>
       </c>
       <c r="L2">
@@ -24812,11 +24812,11 @@
         <v>14</v>
       </c>
       <c r="J3">
-        <f>H3/D3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K3">
-        <f>I3/D3</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L3">
@@ -24856,11 +24856,11 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <f>H4/D4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K4">
-        <f>I4/D4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L4">
@@ -24900,11 +24900,11 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <f>H5/D5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>I5/D5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L5">
@@ -24944,11 +24944,11 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <f>H6/D6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K6">
-        <f>I6/D6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L6">
@@ -24988,11 +24988,11 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <f>H7/D7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K7">
-        <f>I7/D7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L7">
@@ -25032,11 +25032,11 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <f>H8/D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f>I8/D8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L8">
@@ -25076,11 +25076,11 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <f>H9/D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f>I9/D9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L9">
@@ -25173,11 +25173,11 @@
         <v>23.871431324487101</v>
       </c>
       <c r="J13">
-        <f>H13/D13</f>
+        <f t="shared" ref="J13:J20" si="2">H13/D13</f>
         <v>1.2090614410192</v>
       </c>
       <c r="K13">
-        <f>I13/D13</f>
+        <f t="shared" ref="K13:K20" si="3">I13/D13</f>
         <v>1.7051022374633644</v>
       </c>
       <c r="L13">
@@ -25217,11 +25217,11 @@
         <v>22.366350354902501</v>
       </c>
       <c r="J14">
-        <f>H14/D14</f>
+        <f t="shared" si="2"/>
         <v>1.1769091078431715</v>
       </c>
       <c r="K14">
-        <f>I14/D14</f>
+        <f t="shared" si="3"/>
         <v>1.5975964539216072</v>
       </c>
       <c r="L14">
@@ -25261,11 +25261,11 @@
         <v>21.7101393218765</v>
       </c>
       <c r="J15">
-        <f>H15/D15</f>
+        <f t="shared" si="2"/>
         <v>1.1665666842331142</v>
       </c>
       <c r="K15">
-        <f>I15/D15</f>
+        <f t="shared" si="3"/>
         <v>1.5507242372768928</v>
       </c>
       <c r="L15">
@@ -25305,11 +25305,11 @@
         <v>21.8214483787694</v>
       </c>
       <c r="J16">
-        <f>H16/D16</f>
+        <f t="shared" si="2"/>
         <v>1.1717332356871428</v>
       </c>
       <c r="K16">
-        <f>I16/D16</f>
+        <f t="shared" si="3"/>
         <v>1.5586748841978142</v>
       </c>
       <c r="L16">
@@ -25349,11 +25349,11 @@
         <v>22.002552756177899</v>
       </c>
       <c r="J17">
-        <f>H17/D17</f>
+        <f t="shared" si="2"/>
         <v>1.1731562483276572</v>
       </c>
       <c r="K17">
-        <f>I17/D17</f>
+        <f t="shared" si="3"/>
         <v>1.5716109111555643</v>
       </c>
       <c r="L17">
@@ -25393,11 +25393,11 @@
         <v>22.0551733917444</v>
       </c>
       <c r="J18">
-        <f>H18/D18</f>
+        <f t="shared" si="2"/>
         <v>1.1724757152287213</v>
       </c>
       <c r="K18">
-        <f>I18/D18</f>
+        <f t="shared" si="3"/>
         <v>1.5753695279817428</v>
       </c>
       <c r="L18">
@@ -25437,11 +25437,11 @@
         <v>21.868914103434001</v>
       </c>
       <c r="J19">
-        <f>H19/D19</f>
+        <f t="shared" si="2"/>
         <v>1.1601522923399143</v>
       </c>
       <c r="K19">
-        <f>I19/D19</f>
+        <f t="shared" si="3"/>
         <v>1.5620652931024286</v>
       </c>
       <c r="L19">
@@ -25481,11 +25481,11 @@
         <v>21.260399016930698</v>
       </c>
       <c r="J20">
-        <f>H20/D20</f>
+        <f t="shared" si="2"/>
         <v>1.1415937041513</v>
       </c>
       <c r="K20">
-        <f>I20/D20</f>
+        <f t="shared" si="3"/>
         <v>1.5185999297807642</v>
       </c>
       <c r="L20">
@@ -25578,11 +25578,11 @@
         <v>20.815263594371501</v>
       </c>
       <c r="J24">
-        <f>H24/D24</f>
+        <f t="shared" ref="J24:J31" si="4">H24/D24</f>
         <v>1.1313605897368142</v>
       </c>
       <c r="K24">
-        <f>I24/D24</f>
+        <f t="shared" ref="K24:K31" si="5">I24/D24</f>
         <v>1.4868045424551073</v>
       </c>
       <c r="L24">
@@ -25622,11 +25622,11 @@
         <v>21.065339403189501</v>
       </c>
       <c r="J25">
-        <f>H25/D25</f>
+        <f t="shared" si="4"/>
         <v>1.1357078207519</v>
       </c>
       <c r="K25">
-        <f>I25/D25</f>
+        <f t="shared" si="5"/>
         <v>1.5046671002278216</v>
       </c>
       <c r="L25">
@@ -25666,11 +25666,11 @@
         <v>20.0250645390282</v>
       </c>
       <c r="J26">
-        <f>H26/D26</f>
+        <f t="shared" si="4"/>
         <v>1.1150178440634213</v>
       </c>
       <c r="K26">
-        <f>I26/D26</f>
+        <f t="shared" si="5"/>
         <v>1.4303617527877286</v>
       </c>
       <c r="L26">
@@ -25710,11 +25710,11 @@
         <v>20.286720270593001</v>
       </c>
       <c r="J27">
-        <f>H27/D27</f>
+        <f t="shared" si="4"/>
         <v>1.1087283870765285</v>
       </c>
       <c r="K27">
-        <f>I27/D27</f>
+        <f t="shared" si="5"/>
         <v>1.4490514478995</v>
       </c>
       <c r="L27">
@@ -25754,11 +25754,11 @@
         <v>19.956840001875499</v>
       </c>
       <c r="J28">
-        <f>H28/D28</f>
+        <f t="shared" si="4"/>
         <v>1.1071390003855857</v>
       </c>
       <c r="K28">
-        <f>I28/D28</f>
+        <f t="shared" si="5"/>
         <v>1.4254885715625356</v>
       </c>
       <c r="L28">
@@ -25798,11 +25798,11 @@
         <v>20.129539865664999</v>
       </c>
       <c r="J29">
-        <f>H29/D29</f>
+        <f t="shared" si="4"/>
         <v>1.1023804733481</v>
       </c>
       <c r="K29">
-        <f>I29/D29</f>
+        <f t="shared" si="5"/>
         <v>1.4378242761189284</v>
       </c>
       <c r="L29">
@@ -25842,11 +25842,11 @@
         <v>19.483402961131301</v>
       </c>
       <c r="J30">
-        <f>H30/D30</f>
+        <f t="shared" si="4"/>
         <v>1.0783475390855144</v>
       </c>
       <c r="K30">
-        <f>I30/D30</f>
+        <f t="shared" si="5"/>
         <v>1.3916716400808071</v>
       </c>
       <c r="L30">
@@ -25886,11 +25886,11 @@
         <v>19.398042606889099</v>
       </c>
       <c r="J31">
-        <f>H31/D31</f>
+        <f t="shared" si="4"/>
         <v>1.0755511490184213</v>
       </c>
       <c r="K31">
-        <f>I31/D31</f>
+        <f t="shared" si="5"/>
         <v>1.38557447192065</v>
       </c>
       <c r="L31">
@@ -25983,11 +25983,11 @@
         <v>21.494738599220199</v>
       </c>
       <c r="J35">
-        <f>H35/D35</f>
+        <f t="shared" ref="J35:J42" si="6">H35/D35</f>
         <v>1.1295470338992786</v>
       </c>
       <c r="K35">
-        <f>I35/D35</f>
+        <f t="shared" ref="K35:K42" si="7">I35/D35</f>
         <v>1.5353384713728713</v>
       </c>
       <c r="L35">
@@ -26027,11 +26027,11 @@
         <v>21.5254833411961</v>
       </c>
       <c r="J36">
-        <f>H36/D36</f>
+        <f t="shared" si="6"/>
         <v>1.1294120753865287</v>
       </c>
       <c r="K36">
-        <f>I36/D36</f>
+        <f t="shared" si="7"/>
         <v>1.53753452437115</v>
       </c>
       <c r="L36">
@@ -26071,11 +26071,11 @@
         <v>20.987343805984501</v>
       </c>
       <c r="J37">
-        <f>H37/D37</f>
+        <f t="shared" si="6"/>
         <v>1.1292348321956929</v>
       </c>
       <c r="K37">
-        <f>I37/D37</f>
+        <f t="shared" si="7"/>
         <v>1.4990959861417501</v>
       </c>
       <c r="L37">
@@ -26115,11 +26115,11 @@
         <v>21.026233246098599</v>
       </c>
       <c r="J38">
-        <f>H38/D38</f>
+        <f t="shared" si="6"/>
         <v>1.1317586514852214</v>
       </c>
       <c r="K38">
-        <f>I38/D38</f>
+        <f t="shared" si="7"/>
         <v>1.501873803292757</v>
       </c>
       <c r="L38">
@@ -26159,11 +26159,11 @@
         <v>21.0790945889188</v>
       </c>
       <c r="J39">
-        <f>H39/D39</f>
+        <f t="shared" si="6"/>
         <v>1.1324711303888786</v>
       </c>
       <c r="K39">
-        <f>I39/D39</f>
+        <f t="shared" si="7"/>
         <v>1.5056496134941999</v>
       </c>
       <c r="L39">
@@ -26203,11 +26203,11 @@
         <v>21.153273864136999</v>
       </c>
       <c r="J40">
-        <f>H40/D40</f>
+        <f t="shared" si="6"/>
         <v>1.1353164403260643</v>
       </c>
       <c r="K40">
-        <f>I40/D40</f>
+        <f t="shared" si="7"/>
         <v>1.5109481331526429</v>
       </c>
       <c r="L40">
@@ -26247,11 +26247,11 @@
         <v>21.0171662807549</v>
       </c>
       <c r="J41">
-        <f>H41/D41</f>
+        <f t="shared" si="6"/>
         <v>1.1281060818632784</v>
       </c>
       <c r="K41">
-        <f>I41/D41</f>
+        <f t="shared" si="7"/>
         <v>1.5012261629110644</v>
       </c>
       <c r="L41">
@@ -26291,11 +26291,11 @@
         <v>20.923832162899298</v>
       </c>
       <c r="J42">
-        <f>H42/D42</f>
+        <f t="shared" si="6"/>
         <v>1.1136850055105285</v>
       </c>
       <c r="K42">
-        <f>I42/D42</f>
+        <f t="shared" si="7"/>
         <v>1.4945594402070927</v>
       </c>
       <c r="L42">
@@ -26388,11 +26388,11 @@
         <v>14.286084789338901</v>
       </c>
       <c r="J46">
-        <f>H46/D46</f>
+        <f t="shared" ref="J46:J54" si="8">H46/D46</f>
         <v>1.0020827111481858</v>
       </c>
       <c r="K46">
-        <f>I46/D46</f>
+        <f t="shared" ref="K46:K54" si="9">I46/D46</f>
         <v>1.0204346278099214</v>
       </c>
       <c r="L46">
@@ -26432,11 +26432,11 @@
         <v>14.9952362786352</v>
       </c>
       <c r="J47">
-        <f>H47/D47</f>
+        <f t="shared" si="8"/>
         <v>1.0075693229322857</v>
       </c>
       <c r="K47">
-        <f>I47/D47</f>
+        <f t="shared" si="9"/>
         <v>1.0710883056168001</v>
       </c>
       <c r="L47">
@@ -26476,11 +26476,11 @@
         <v>14.946443509293999</v>
       </c>
       <c r="J48">
-        <f>H48/D48</f>
+        <f t="shared" si="8"/>
         <v>1.0073453663128284</v>
       </c>
       <c r="K48">
-        <f>I48/D48</f>
+        <f t="shared" si="9"/>
         <v>1.0676031078067143</v>
       </c>
       <c r="L48">
@@ -26520,11 +26520,11 @@
         <v>14.9543446942915</v>
       </c>
       <c r="J49">
-        <f>H49/D49</f>
+        <f t="shared" si="8"/>
         <v>1.0076021580980856</v>
       </c>
       <c r="K49">
-        <f>I49/D49</f>
+        <f t="shared" si="9"/>
         <v>1.0681674781636785</v>
       </c>
       <c r="L49">
@@ -26564,11 +26564,11 @@
         <v>15.206083867268299</v>
       </c>
       <c r="J50">
-        <f>H50/D50</f>
+        <f t="shared" si="8"/>
         <v>1.0098596131537214</v>
       </c>
       <c r="K50">
-        <f>I50/D50</f>
+        <f t="shared" si="9"/>
         <v>1.0861488476620214</v>
       </c>
       <c r="L50">
@@ -26608,11 +26608,11 @@
         <v>15.2651696129338</v>
       </c>
       <c r="J51">
-        <f>H51/D51</f>
+        <f t="shared" si="8"/>
         <v>1.0102769961358213</v>
       </c>
       <c r="K51">
-        <f>I51/D51</f>
+        <f t="shared" si="9"/>
         <v>1.0903692580666999</v>
       </c>
       <c r="L51">
@@ -26652,11 +26652,11 @@
         <v>15.4769378263427</v>
       </c>
       <c r="J52">
-        <f>H52/D52</f>
+        <f t="shared" si="8"/>
         <v>1.0125397993166143</v>
       </c>
       <c r="K52">
-        <f>I52/D52</f>
+        <f t="shared" si="9"/>
         <v>1.1054955590244786</v>
       </c>
       <c r="L52">
@@ -26696,11 +26696,11 @@
         <v>15.2661124434618</v>
       </c>
       <c r="J53">
-        <f>H53/D53</f>
+        <f t="shared" si="8"/>
         <v>1.0104348712110143</v>
       </c>
       <c r="K53">
-        <f>I53/D53</f>
+        <f t="shared" si="9"/>
         <v>1.0904366031044144</v>
       </c>
       <c r="L53">
@@ -26740,11 +26740,11 @@
         <v>15.530207131494601</v>
       </c>
       <c r="J54">
-        <f>H54/D54</f>
+        <f t="shared" si="8"/>
         <v>1.0122323743127644</v>
       </c>
       <c r="K54">
-        <f>I54/D54</f>
+        <f t="shared" si="9"/>
         <v>1.1093005093924715</v>
       </c>
       <c r="L54">
@@ -26769,8 +26769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51076D5-8C47-466A-ADDA-1B7F4F91417B}">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:M54"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26858,11 +26858,11 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <f>H2/D2</f>
+        <f t="shared" ref="J2:J9" si="0">H2/D2</f>
         <v>1</v>
       </c>
       <c r="K2">
-        <f>I2/D2</f>
+        <f t="shared" ref="K2:K9" si="1">I2/D2</f>
         <v>1</v>
       </c>
       <c r="L2">
@@ -26902,11 +26902,11 @@
         <v>14</v>
       </c>
       <c r="J3">
-        <f>H3/D3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K3">
-        <f>I3/D3</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L3">
@@ -26946,11 +26946,11 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <f>H4/D4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K4">
-        <f>I4/D4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L4">
@@ -26990,11 +26990,11 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <f>H5/D5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>I5/D5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L5">
@@ -27034,11 +27034,11 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <f>H6/D6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K6">
-        <f>I6/D6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L6">
@@ -27078,11 +27078,11 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <f>H7/D7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K7">
-        <f>I7/D7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L7">
@@ -27122,11 +27122,11 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <f>H8/D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f>I8/D8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L8">
@@ -27166,11 +27166,11 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <f>H9/D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f>I9/D9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L9">
@@ -27263,11 +27263,11 @@
         <v>21.7293418749375</v>
       </c>
       <c r="J13">
-        <f>H13/D13</f>
+        <f t="shared" ref="J13:J21" si="2">H13/D13</f>
         <v>1.158040360953557</v>
       </c>
       <c r="K13">
-        <f>I13/D13</f>
+        <f t="shared" ref="K13:K21" si="3">I13/D13</f>
         <v>1.5520958482098215</v>
       </c>
       <c r="L13">
@@ -27307,11 +27307,11 @@
         <v>20.8068930769657</v>
       </c>
       <c r="J14">
-        <f>H14/D14</f>
+        <f t="shared" si="2"/>
         <v>1.1416954608265786</v>
       </c>
       <c r="K14">
-        <f>I14/D14</f>
+        <f t="shared" si="3"/>
         <v>1.486206648354693</v>
       </c>
       <c r="L14">
@@ -27351,11 +27351,11 @@
         <v>20.000053566518801</v>
       </c>
       <c r="J15">
-        <f>H15/D15</f>
+        <f t="shared" si="2"/>
         <v>1.1336262837021642</v>
       </c>
       <c r="K15">
-        <f>I15/D15</f>
+        <f t="shared" si="3"/>
         <v>1.4285752547513428</v>
       </c>
       <c r="L15">
@@ -27395,11 +27395,11 @@
         <v>20.233263579375102</v>
       </c>
       <c r="J16">
-        <f>H16/D16</f>
+        <f t="shared" si="2"/>
         <v>1.1331839460571143</v>
       </c>
       <c r="K16">
-        <f>I16/D16</f>
+        <f t="shared" si="3"/>
         <v>1.4452331128125073</v>
       </c>
       <c r="L16">
@@ -27439,11 +27439,11 @@
         <v>20.2671960661295</v>
       </c>
       <c r="J17">
-        <f>H17/D17</f>
+        <f t="shared" si="2"/>
         <v>1.137162058455</v>
       </c>
       <c r="K17">
-        <f>I17/D17</f>
+        <f t="shared" si="3"/>
         <v>1.447656861866393</v>
       </c>
       <c r="L17">
@@ -27483,11 +27483,11 @@
         <v>20.403074724176602</v>
       </c>
       <c r="J18">
-        <f>H18/D18</f>
+        <f t="shared" si="2"/>
         <v>1.1353845824443358</v>
       </c>
       <c r="K18">
-        <f>I18/D18</f>
+        <f t="shared" si="3"/>
         <v>1.4573624802983287</v>
       </c>
       <c r="L18">
@@ -27527,11 +27527,11 @@
         <v>20.1455101359143</v>
       </c>
       <c r="J19">
-        <f>H19/D19</f>
+        <f t="shared" si="2"/>
         <v>1.1239441451804999</v>
       </c>
       <c r="K19">
-        <f>I19/D19</f>
+        <f t="shared" si="3"/>
         <v>1.4389650097081643</v>
       </c>
       <c r="L19">
@@ -27571,11 +27571,11 @@
         <v>19.776722480829498</v>
       </c>
       <c r="J20">
-        <f>H20/D20</f>
+        <f t="shared" si="2"/>
         <v>1.1100752813643857</v>
       </c>
       <c r="K20">
-        <f>I20/D20</f>
+        <f t="shared" si="3"/>
         <v>1.4126230343449642</v>
       </c>
       <c r="L20">
@@ -27597,11 +27597,11 @@
         <v>2500</v>
       </c>
       <c r="J21" t="e">
-        <f>H21/D21</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K21" t="e">
-        <f>I21/D21</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -27676,11 +27676,11 @@
         <v>19.536080316529901</v>
       </c>
       <c r="J24">
-        <f>H24/D24</f>
+        <f t="shared" ref="J24:J32" si="4">H24/D24</f>
         <v>1.1152244331529857</v>
       </c>
       <c r="K24">
-        <f>I24/D24</f>
+        <f t="shared" ref="K24:K32" si="5">I24/D24</f>
         <v>1.3954343083235643</v>
       </c>
       <c r="L24">
@@ -27720,11 +27720,11 @@
         <v>19.617495548369298</v>
       </c>
       <c r="J25">
-        <f>H25/D25</f>
+        <f t="shared" si="4"/>
         <v>1.1112746739776571</v>
       </c>
       <c r="K25">
-        <f>I25/D25</f>
+        <f t="shared" si="5"/>
         <v>1.4012496820263785</v>
       </c>
       <c r="L25">
@@ -27764,11 +27764,11 @@
         <v>19.206144142728501</v>
       </c>
       <c r="J26">
-        <f>H26/D26</f>
+        <f t="shared" si="4"/>
         <v>1.0986407307426429</v>
       </c>
       <c r="K26">
-        <f>I26/D26</f>
+        <f t="shared" si="5"/>
         <v>1.3718674387663214</v>
       </c>
       <c r="L26">
@@ -27808,11 +27808,11 @@
         <v>19.409650017463001</v>
       </c>
       <c r="J27">
-        <f>H27/D27</f>
+        <f t="shared" si="4"/>
         <v>1.0989414622490357</v>
       </c>
       <c r="K27">
-        <f>I27/D27</f>
+        <f t="shared" si="5"/>
         <v>1.3864035726759287</v>
       </c>
       <c r="L27">
@@ -27852,11 +27852,11 @@
         <v>19.1909322366791</v>
       </c>
       <c r="J28">
-        <f>H28/D28</f>
+        <f t="shared" si="4"/>
         <v>1.0969394612585928</v>
       </c>
       <c r="K28">
-        <f>I28/D28</f>
+        <f t="shared" si="5"/>
         <v>1.370780874048507</v>
       </c>
       <c r="L28">
@@ -27896,11 +27896,11 @@
         <v>19.2262547050025</v>
       </c>
       <c r="J29">
-        <f>H29/D29</f>
+        <f t="shared" si="4"/>
         <v>1.0937492493972356</v>
       </c>
       <c r="K29">
-        <f>I29/D29</f>
+        <f t="shared" si="5"/>
         <v>1.3733039075001785</v>
       </c>
       <c r="L29">
@@ -27940,11 +27940,11 @@
         <v>18.6362815571607</v>
       </c>
       <c r="J30">
-        <f>H30/D30</f>
+        <f t="shared" si="4"/>
         <v>1.0726470038186287</v>
       </c>
       <c r="K30">
-        <f>I30/D30</f>
+        <f t="shared" si="5"/>
         <v>1.3311629683686215</v>
       </c>
       <c r="L30">
@@ -27984,11 +27984,11 @@
         <v>18.5434780204905</v>
       </c>
       <c r="J31">
-        <f>H31/D31</f>
+        <f t="shared" si="4"/>
         <v>1.0699839512425287</v>
       </c>
       <c r="K31">
-        <f>I31/D31</f>
+        <f t="shared" si="5"/>
         <v>1.3245341443207501</v>
       </c>
       <c r="L31">
@@ -28010,11 +28010,11 @@
         <v>2500</v>
       </c>
       <c r="J32" t="e">
-        <f>H32/D32</f>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K32" t="e">
-        <f>I32/D32</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -28089,11 +28089,11 @@
         <v>20.018994089070699</v>
       </c>
       <c r="J35">
-        <f>H35/D35</f>
+        <f t="shared" ref="J35:J43" si="6">H35/D35</f>
         <v>1.1069004681818428</v>
       </c>
       <c r="K35">
-        <f>I35/D35</f>
+        <f t="shared" ref="K35:K43" si="7">I35/D35</f>
         <v>1.4299281492193356</v>
       </c>
       <c r="L35">
@@ -28133,11 +28133,11 @@
         <v>20.2763365104028</v>
       </c>
       <c r="J36">
-        <f>H36/D36</f>
+        <f t="shared" si="6"/>
         <v>1.1086774861128144</v>
       </c>
       <c r="K36">
-        <f>I36/D36</f>
+        <f t="shared" si="7"/>
         <v>1.4483097507430571</v>
       </c>
       <c r="L36">
@@ -28177,11 +28177,11 @@
         <v>19.488167117154099</v>
       </c>
       <c r="J37">
-        <f>H37/D37</f>
+        <f t="shared" si="6"/>
         <v>1.100760953808043</v>
       </c>
       <c r="K37">
-        <f>I37/D37</f>
+        <f t="shared" si="7"/>
         <v>1.3920119369395785</v>
       </c>
       <c r="L37">
@@ -28221,11 +28221,11 @@
         <v>19.4658406286276</v>
       </c>
       <c r="J38">
-        <f>H38/D38</f>
+        <f t="shared" si="6"/>
         <v>1.1006074553890857</v>
       </c>
       <c r="K38">
-        <f>I38/D38</f>
+        <f t="shared" si="7"/>
         <v>1.3904171877591143</v>
       </c>
       <c r="L38">
@@ -28265,11 +28265,11 @@
         <v>19.834724764991901</v>
       </c>
       <c r="J39">
-        <f>H39/D39</f>
+        <f t="shared" si="6"/>
         <v>1.1089188000319428</v>
       </c>
       <c r="K39">
-        <f>I39/D39</f>
+        <f t="shared" si="7"/>
         <v>1.4167660546422787</v>
       </c>
       <c r="L39">
@@ -28309,11 +28309,11 @@
         <v>19.891860720335799</v>
       </c>
       <c r="J40">
-        <f>H40/D40</f>
+        <f t="shared" si="6"/>
         <v>1.1126101737866929</v>
       </c>
       <c r="K40">
-        <f>I40/D40</f>
+        <f t="shared" si="7"/>
         <v>1.4208471943096999</v>
       </c>
       <c r="L40">
@@ -28353,11 +28353,11 @@
         <v>19.488607050257801</v>
       </c>
       <c r="J41">
-        <f>H41/D41</f>
+        <f t="shared" si="6"/>
         <v>1.0987085667974643</v>
       </c>
       <c r="K41">
-        <f>I41/D41</f>
+        <f t="shared" si="7"/>
         <v>1.3920433607327001</v>
       </c>
       <c r="L41">
@@ -28397,11 +28397,11 @@
         <v>19.097404443669301</v>
       </c>
       <c r="J42">
-        <f>H42/D42</f>
+        <f t="shared" si="6"/>
         <v>1.0838555563386214</v>
       </c>
       <c r="K42">
-        <f>I42/D42</f>
+        <f t="shared" si="7"/>
         <v>1.3641003174049502</v>
       </c>
       <c r="L42">
@@ -28423,11 +28423,11 @@
         <v>2500</v>
       </c>
       <c r="J43" t="e">
-        <f>H43/D43</f>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K43" t="e">
-        <f>I43/D43</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -28502,11 +28502,11 @@
         <v>14.286084789338901</v>
       </c>
       <c r="J46">
-        <f>H46/D46</f>
+        <f t="shared" ref="J46:J54" si="8">H46/D46</f>
         <v>1.0020827111481858</v>
       </c>
       <c r="K46">
-        <f>I46/D46</f>
+        <f t="shared" ref="K46:K54" si="9">I46/D46</f>
         <v>1.0204346278099214</v>
       </c>
       <c r="L46">
@@ -28546,11 +28546,11 @@
         <v>14.9952362786352</v>
       </c>
       <c r="J47">
-        <f>H47/D47</f>
+        <f t="shared" si="8"/>
         <v>1.0075693229322857</v>
       </c>
       <c r="K47">
-        <f>I47/D47</f>
+        <f t="shared" si="9"/>
         <v>1.0710883056168001</v>
       </c>
       <c r="L47">
@@ -28590,11 +28590,11 @@
         <v>14.946443509293999</v>
       </c>
       <c r="J48">
-        <f>H48/D48</f>
+        <f t="shared" si="8"/>
         <v>1.0073453663128284</v>
       </c>
       <c r="K48">
-        <f>I48/D48</f>
+        <f t="shared" si="9"/>
         <v>1.0676031078067143</v>
       </c>
       <c r="L48">
@@ -28634,11 +28634,11 @@
         <v>14.9511552184461</v>
       </c>
       <c r="J49">
-        <f>H49/D49</f>
+        <f t="shared" si="8"/>
         <v>1.0075547441138144</v>
       </c>
       <c r="K49">
-        <f>I49/D49</f>
+        <f t="shared" si="9"/>
         <v>1.0679396584604357</v>
       </c>
       <c r="L49">
@@ -28678,11 +28678,11 @@
         <v>15.1673201771075</v>
       </c>
       <c r="J50">
-        <f>H50/D50</f>
+        <f t="shared" si="8"/>
         <v>1.0095824378691929</v>
       </c>
       <c r="K50">
-        <f>I50/D50</f>
+        <f t="shared" si="9"/>
         <v>1.0833800126505357</v>
       </c>
       <c r="L50">
@@ -28722,11 +28722,11 @@
         <v>15.228665338078599</v>
       </c>
       <c r="J51">
-        <f>H51/D51</f>
+        <f t="shared" si="8"/>
         <v>1.0099981258910786</v>
       </c>
       <c r="K51">
-        <f>I51/D51</f>
+        <f t="shared" si="9"/>
         <v>1.0877618098627571</v>
       </c>
       <c r="L51">
@@ -28766,11 +28766,11 @@
         <v>15.436981297344101</v>
       </c>
       <c r="J52">
-        <f>H52/D52</f>
+        <f t="shared" si="8"/>
         <v>1.0123293500457644</v>
       </c>
       <c r="K52">
-        <f>I52/D52</f>
+        <f t="shared" si="9"/>
         <v>1.1026415212388643</v>
       </c>
       <c r="L52">
@@ -28810,11 +28810,11 @@
         <v>15.242758930074899</v>
       </c>
       <c r="J53">
-        <f>H53/D53</f>
+        <f t="shared" si="8"/>
         <v>1.0102614056036929</v>
       </c>
       <c r="K53">
-        <f>I53/D53</f>
+        <f t="shared" si="9"/>
         <v>1.08876849500535</v>
       </c>
       <c r="L53">
@@ -28836,11 +28836,11 @@
         <v>2500</v>
       </c>
       <c r="J54" t="e">
-        <f>H54/D54</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K54" t="e">
-        <f>I54/D54</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -28951,11 +28951,11 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <f>H2/D2</f>
+        <f t="shared" ref="J2:J10" si="0">H2/D2</f>
         <v>1</v>
       </c>
       <c r="K2">
-        <f>I2/D2</f>
+        <f t="shared" ref="K2:K10" si="1">I2/D2</f>
         <v>1</v>
       </c>
       <c r="L2">
@@ -28995,11 +28995,11 @@
         <v>14</v>
       </c>
       <c r="J3">
-        <f>H3/D3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K3">
-        <f>I3/D3</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L3">
@@ -29039,11 +29039,11 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <f>H4/D4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K4">
-        <f>I4/D4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L4">
@@ -29083,11 +29083,11 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <f>H5/D5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>I5/D5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L5">
@@ -29127,11 +29127,11 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <f>H6/D6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K6">
-        <f>I6/D6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L6">
@@ -29171,11 +29171,11 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <f>H7/D7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K7">
-        <f>I7/D7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L7">
@@ -29215,11 +29215,11 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <f>H8/D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f>I8/D8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L8">
@@ -29259,11 +29259,11 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <f>H9/D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f>I9/D9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L9">
@@ -29303,11 +29303,11 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <f>H10/D10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K10">
-        <f>I10/D10</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L10">
@@ -29388,11 +29388,11 @@
         <v>20.609498382411001</v>
       </c>
       <c r="J13">
-        <f>H13/D13</f>
+        <f t="shared" ref="J13:J21" si="2">H13/D13</f>
         <v>1.1239230877234072</v>
       </c>
       <c r="K13">
-        <f>I13/D13</f>
+        <f t="shared" ref="K13:K21" si="3">I13/D13</f>
         <v>1.4721070273150716</v>
       </c>
       <c r="L13">
@@ -29432,11 +29432,11 @@
         <v>20.091176892683599</v>
       </c>
       <c r="J14">
-        <f>H14/D14</f>
+        <f t="shared" si="2"/>
         <v>1.1121680401703786</v>
       </c>
       <c r="K14">
-        <f>I14/D14</f>
+        <f t="shared" si="3"/>
         <v>1.4350840637631141</v>
       </c>
       <c r="L14">
@@ -29476,11 +29476,11 @@
         <v>19.700088807527099</v>
       </c>
       <c r="J15">
-        <f>H15/D15</f>
+        <f t="shared" si="2"/>
         <v>1.1069231734084286</v>
       </c>
       <c r="K15">
-        <f>I15/D15</f>
+        <f t="shared" si="3"/>
         <v>1.4071492005376498</v>
       </c>
       <c r="L15">
@@ -29520,11 +29520,11 @@
         <v>19.602519965750702</v>
       </c>
       <c r="J16">
-        <f>H16/D16</f>
+        <f t="shared" si="2"/>
         <v>1.1044342572123571</v>
       </c>
       <c r="K16">
-        <f>I16/D16</f>
+        <f t="shared" si="3"/>
         <v>1.4001799975536215</v>
       </c>
       <c r="L16">
@@ -29564,11 +29564,11 @@
         <v>19.645792993240601</v>
       </c>
       <c r="J17">
-        <f>H17/D17</f>
+        <f t="shared" si="2"/>
         <v>1.1098213731443214</v>
       </c>
       <c r="K17">
-        <f>I17/D17</f>
+        <f t="shared" si="3"/>
         <v>1.4032709280886144</v>
       </c>
       <c r="L17">
@@ -29608,11 +29608,11 @@
         <v>19.897068490632201</v>
       </c>
       <c r="J18">
-        <f>H18/D18</f>
+        <f t="shared" si="2"/>
         <v>1.1061112678672858</v>
       </c>
       <c r="K18">
-        <f>I18/D18</f>
+        <f t="shared" si="3"/>
         <v>1.4212191779023</v>
       </c>
       <c r="L18">
@@ -29652,11 +29652,11 @@
         <v>19.769812515039799</v>
       </c>
       <c r="J19">
-        <f>H19/D19</f>
+        <f t="shared" si="2"/>
         <v>1.10165976423675</v>
       </c>
       <c r="K19">
-        <f>I19/D19</f>
+        <f t="shared" si="3"/>
         <v>1.4121294653599856</v>
       </c>
       <c r="L19">
@@ -29696,11 +29696,11 @@
         <v>19.331560028726699</v>
       </c>
       <c r="J20">
-        <f>H20/D20</f>
+        <f t="shared" si="2"/>
         <v>1.0865851355394858</v>
       </c>
       <c r="K20">
-        <f>I20/D20</f>
+        <f t="shared" si="3"/>
         <v>1.3808257163376214</v>
       </c>
       <c r="L20">
@@ -29740,11 +29740,11 @@
         <v>27.733681490398801</v>
       </c>
       <c r="J21">
-        <f>H21/D21</f>
+        <f t="shared" si="2"/>
         <v>1.1649218422088428</v>
       </c>
       <c r="K21">
-        <f>I21/D21</f>
+        <f t="shared" si="3"/>
         <v>1.9809772493142002</v>
       </c>
       <c r="L21">
@@ -29825,11 +29825,11 @@
         <v>19.8529257685502</v>
       </c>
       <c r="J24">
-        <f>H24/D24</f>
+        <f t="shared" ref="J24:J32" si="4">H24/D24</f>
         <v>1.1011876219588144</v>
       </c>
       <c r="K24">
-        <f>I24/D24</f>
+        <f t="shared" ref="K24:K32" si="5">I24/D24</f>
         <v>1.4180661263250143</v>
       </c>
       <c r="L24">
@@ -29869,11 +29869,11 @@
         <v>19.6486788886439</v>
       </c>
       <c r="J25">
-        <f>H25/D25</f>
+        <f t="shared" si="4"/>
         <v>1.0941165395757499</v>
       </c>
       <c r="K25">
-        <f>I25/D25</f>
+        <f t="shared" si="5"/>
         <v>1.4034770634745644</v>
       </c>
       <c r="L25">
@@ -29913,11 +29913,11 @@
         <v>18.6678945069586</v>
       </c>
       <c r="J26">
-        <f>H26/D26</f>
+        <f t="shared" si="4"/>
         <v>1.0830587238612714</v>
       </c>
       <c r="K26">
-        <f>I26/D26</f>
+        <f t="shared" si="5"/>
         <v>1.3334210362113286</v>
       </c>
       <c r="L26">
@@ -29957,11 +29957,11 @@
         <v>19.159971814190499</v>
       </c>
       <c r="J27">
-        <f>H27/D27</f>
+        <f t="shared" si="4"/>
         <v>1.0825396164949714</v>
       </c>
       <c r="K27">
-        <f>I27/D27</f>
+        <f t="shared" si="5"/>
         <v>1.3685694152993213</v>
       </c>
       <c r="L27">
@@ -30001,11 +30001,11 @@
         <v>18.904438639762802</v>
       </c>
       <c r="J28">
-        <f>H28/D28</f>
+        <f t="shared" si="4"/>
         <v>1.0815777714158357</v>
       </c>
       <c r="K28">
-        <f>I28/D28</f>
+        <f t="shared" si="5"/>
         <v>1.350317045697343</v>
       </c>
       <c r="L28">
@@ -30045,11 +30045,11 @@
         <v>18.737359153661799</v>
       </c>
       <c r="J29">
-        <f>H29/D29</f>
+        <f t="shared" si="4"/>
         <v>1.0791481061371</v>
       </c>
       <c r="K29">
-        <f>I29/D29</f>
+        <f t="shared" si="5"/>
         <v>1.3383827966901285</v>
       </c>
       <c r="L29">
@@ -30089,11 +30089,11 @@
         <v>18.247433862611</v>
       </c>
       <c r="J30">
-        <f>H30/D30</f>
+        <f t="shared" si="4"/>
         <v>1.0631151577973357</v>
       </c>
       <c r="K30">
-        <f>I30/D30</f>
+        <f t="shared" si="5"/>
         <v>1.303388133043643</v>
       </c>
       <c r="L30">
@@ -30133,11 +30133,11 @@
         <v>18.291195114072</v>
       </c>
       <c r="J31">
-        <f>H31/D31</f>
+        <f t="shared" si="4"/>
         <v>1.0626644149462714</v>
       </c>
       <c r="K31">
-        <f>I31/D31</f>
+        <f t="shared" si="5"/>
         <v>1.3065139367194285</v>
       </c>
       <c r="L31">
@@ -30177,11 +30177,11 @@
         <v>17.6528813456808</v>
       </c>
       <c r="J32">
-        <f>H32/D32</f>
+        <f t="shared" si="4"/>
         <v>1.0493003408774499</v>
       </c>
       <c r="K32">
-        <f>I32/D32</f>
+        <f t="shared" si="5"/>
         <v>1.2609200961200571</v>
       </c>
       <c r="L32">
@@ -30262,11 +30262,11 @@
         <v>19.182705905429199</v>
       </c>
       <c r="J35">
-        <f>H35/D35</f>
+        <f t="shared" ref="J35:J43" si="6">H35/D35</f>
         <v>1.0741837656873356</v>
       </c>
       <c r="K35">
-        <f>I35/D35</f>
+        <f t="shared" ref="K35:K43" si="7">I35/D35</f>
         <v>1.3701932789592284</v>
       </c>
       <c r="L35">
@@ -30306,11 +30306,11 @@
         <v>19.537138874160899</v>
       </c>
       <c r="J36">
-        <f>H36/D36</f>
+        <f t="shared" si="6"/>
         <v>1.0849653813583</v>
       </c>
       <c r="K36">
-        <f>I36/D36</f>
+        <f t="shared" si="7"/>
         <v>1.3955099195829213</v>
       </c>
       <c r="L36">
@@ -30350,11 +30350,11 @@
         <v>19.3172296800278</v>
       </c>
       <c r="J37">
-        <f>H37/D37</f>
+        <f t="shared" si="6"/>
         <v>1.0842585134949501</v>
       </c>
       <c r="K37">
-        <f>I37/D37</f>
+        <f t="shared" si="7"/>
         <v>1.3798021200019857</v>
       </c>
       <c r="L37">
@@ -30394,11 +30394,11 @@
         <v>19.467720592811901</v>
       </c>
       <c r="J38">
-        <f>H38/D38</f>
+        <f t="shared" si="6"/>
         <v>1.0851850132581713</v>
       </c>
       <c r="K38">
-        <f>I38/D38</f>
+        <f t="shared" si="7"/>
         <v>1.3905514709151359</v>
       </c>
       <c r="L38">
@@ -30438,11 +30438,11 @@
         <v>19.548242832860499</v>
       </c>
       <c r="J39">
-        <f>H39/D39</f>
+        <f t="shared" si="6"/>
         <v>1.0890086687673144</v>
       </c>
       <c r="K39">
-        <f>I39/D39</f>
+        <f t="shared" si="7"/>
         <v>1.3963030594900356</v>
       </c>
       <c r="L39">
@@ -30482,11 +30482,11 @@
         <v>19.226200503096901</v>
       </c>
       <c r="J40">
-        <f>H40/D40</f>
+        <f t="shared" si="6"/>
         <v>1.08830686234925</v>
       </c>
       <c r="K40">
-        <f>I40/D40</f>
+        <f t="shared" si="7"/>
         <v>1.373300035935493</v>
       </c>
       <c r="L40">
@@ -30526,11 +30526,11 @@
         <v>18.885989583052002</v>
       </c>
       <c r="J41">
-        <f>H41/D41</f>
+        <f t="shared" si="6"/>
         <v>1.0747771846158358</v>
       </c>
       <c r="K41">
-        <f>I41/D41</f>
+        <f t="shared" si="7"/>
         <v>1.3489992559322859</v>
       </c>
       <c r="L41">
@@ -30570,11 +30570,11 @@
         <v>18.442890205842701</v>
       </c>
       <c r="J42">
-        <f>H42/D42</f>
+        <f t="shared" si="6"/>
         <v>1.0645589059925142</v>
       </c>
       <c r="K42">
-        <f>I42/D42</f>
+        <f t="shared" si="7"/>
         <v>1.3173493004173358</v>
       </c>
       <c r="L42">
@@ -30614,11 +30614,11 @@
         <v>18.489985145435099</v>
       </c>
       <c r="J43">
-        <f>H43/D43</f>
+        <f t="shared" si="6"/>
         <v>1.0668693878989786</v>
       </c>
       <c r="K43">
-        <f>I43/D43</f>
+        <f t="shared" si="7"/>
         <v>1.3207132246739357</v>
       </c>
       <c r="L43">
@@ -30699,11 +30699,11 @@
         <v>14.286084789338901</v>
       </c>
       <c r="J46">
-        <f>H46/D46</f>
+        <f t="shared" ref="J46:J54" si="8">H46/D46</f>
         <v>1.0020827111481858</v>
       </c>
       <c r="K46">
-        <f>I46/D46</f>
+        <f t="shared" ref="K46:K54" si="9">I46/D46</f>
         <v>1.0204346278099214</v>
       </c>
       <c r="L46">
@@ -30743,11 +30743,11 @@
         <v>14.990695733825101</v>
       </c>
       <c r="J47">
-        <f>H47/D47</f>
+        <f t="shared" si="8"/>
         <v>1.0075660449883073</v>
       </c>
       <c r="K47">
-        <f>I47/D47</f>
+        <f t="shared" si="9"/>
         <v>1.0707639809875071</v>
       </c>
       <c r="L47">
@@ -30787,11 +30787,11 @@
         <v>14.923547003511599</v>
       </c>
       <c r="J48">
-        <f>H48/D48</f>
+        <f t="shared" si="8"/>
         <v>1.0071880154953357</v>
       </c>
       <c r="K48">
-        <f>I48/D48</f>
+        <f t="shared" si="9"/>
         <v>1.0659676431079714</v>
       </c>
       <c r="L48">
@@ -30831,11 +30831,11 @@
         <v>15.0161547891576</v>
       </c>
       <c r="J49">
-        <f>H49/D49</f>
+        <f t="shared" si="8"/>
         <v>1.0081162611338643</v>
       </c>
       <c r="K49">
-        <f>I49/D49</f>
+        <f t="shared" si="9"/>
         <v>1.0725824849398287</v>
       </c>
       <c r="L49">
@@ -30875,11 +30875,11 @@
         <v>15.151780484385601</v>
       </c>
       <c r="J50">
-        <f>H50/D50</f>
+        <f t="shared" si="8"/>
         <v>1.0094496048467143</v>
       </c>
       <c r="K50">
-        <f>I50/D50</f>
+        <f t="shared" si="9"/>
         <v>1.0822700345989715</v>
       </c>
       <c r="L50">
@@ -30919,11 +30919,11 @@
         <v>15.215328529166699</v>
       </c>
       <c r="J51">
-        <f>H51/D51</f>
+        <f t="shared" si="8"/>
         <v>1.0099278265867571</v>
       </c>
       <c r="K51">
-        <f>I51/D51</f>
+        <f t="shared" si="9"/>
         <v>1.0868091806547642</v>
       </c>
       <c r="L51">
@@ -30963,11 +30963,11 @@
         <v>15.1895669661198</v>
       </c>
       <c r="J52">
-        <f>H52/D52</f>
+        <f t="shared" si="8"/>
         <v>1.0104127133372713</v>
       </c>
       <c r="K52">
-        <f>I52/D52</f>
+        <f t="shared" si="9"/>
         <v>1.0849690690085572</v>
       </c>
       <c r="L52">
@@ -31007,11 +31007,11 @@
         <v>15.120454533959199</v>
       </c>
       <c r="J53">
-        <f>H53/D53</f>
+        <f t="shared" si="8"/>
         <v>1.0091303212184142</v>
       </c>
       <c r="K53">
-        <f>I53/D53</f>
+        <f t="shared" si="9"/>
         <v>1.0800324667113714</v>
       </c>
       <c r="L53">
@@ -31051,11 +31051,11 @@
         <v>15.282893116596499</v>
       </c>
       <c r="J54">
-        <f>H54/D54</f>
+        <f t="shared" si="8"/>
         <v>1.0105797688755214</v>
       </c>
       <c r="K54">
-        <f>I54/D54</f>
+        <f t="shared" si="9"/>
         <v>1.0916352226140356</v>
       </c>
       <c r="L54">
@@ -31083,8 +31083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A01F083-4FDE-4172-965F-E873009AF47B}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31177,7 +31177,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <f>I2/D2</f>
+        <f t="shared" ref="K2:K10" si="0">I2/D2</f>
         <v>1</v>
       </c>
       <c r="L2">
@@ -31214,11 +31214,11 @@
         <v>14</v>
       </c>
       <c r="J3">
-        <f>H3/D3</f>
+        <f t="shared" ref="J2:J10" si="1">H3/D3</f>
         <v>1</v>
       </c>
       <c r="K3">
-        <f>I3/D3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L3">
@@ -31255,11 +31255,11 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <f>H4/D4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K4">
-        <f>I4/D4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L4">
@@ -31296,11 +31296,11 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <f>H5/D5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>I5/D5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5">
@@ -31337,11 +31337,11 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <f>H6/D6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K6">
-        <f>I6/D6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L6">
@@ -31378,11 +31378,11 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <f>H7/D7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K7">
-        <f>I7/D7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L7">
@@ -31419,11 +31419,11 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <f>H8/D8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f>I8/D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L8">
@@ -31460,11 +31460,11 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <f>H9/D9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f>I9/D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L9">
@@ -31501,11 +31501,11 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <f>H10/D10</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K10">
-        <f>I10/D10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L10">
@@ -31581,11 +31581,11 @@
         <v>19.332969529943998</v>
       </c>
       <c r="J13">
-        <f>H13/D13</f>
+        <f t="shared" ref="J13:J21" si="2">H13/D13</f>
         <v>1.0986144563591285</v>
       </c>
       <c r="K13">
-        <f>I13/D13</f>
+        <f t="shared" ref="K13:K21" si="3">I13/D13</f>
         <v>1.3809263949959998</v>
       </c>
       <c r="L13">
@@ -31622,11 +31622,11 @@
         <v>18.564600509735801</v>
       </c>
       <c r="J14">
-        <f>H14/D14</f>
+        <f t="shared" si="2"/>
         <v>1.0857849143248928</v>
       </c>
       <c r="K14">
-        <f>I14/D14</f>
+        <f t="shared" si="3"/>
         <v>1.3260428935525572</v>
       </c>
       <c r="L14">
@@ -31663,11 +31663,11 @@
         <v>17.9348867366969</v>
       </c>
       <c r="J15">
-        <f>H15/D15</f>
+        <f t="shared" si="2"/>
         <v>1.0756141720272714</v>
       </c>
       <c r="K15">
-        <f>I15/D15</f>
+        <f t="shared" si="3"/>
         <v>1.2810633383354928</v>
       </c>
       <c r="L15">
@@ -31704,11 +31704,11 @@
         <v>17.950950161308601</v>
       </c>
       <c r="J16">
-        <f>H16/D16</f>
+        <f t="shared" si="2"/>
         <v>1.0738652348942999</v>
       </c>
       <c r="K16">
-        <f>I16/D16</f>
+        <f t="shared" si="3"/>
         <v>1.2822107258077573</v>
       </c>
       <c r="L16">
@@ -31745,11 +31745,11 @@
         <v>17.595135243734401</v>
       </c>
       <c r="J17">
-        <f>H17/D17</f>
+        <f t="shared" si="2"/>
         <v>1.0670426008954428</v>
       </c>
       <c r="K17">
-        <f>I17/D17</f>
+        <f t="shared" si="3"/>
         <v>1.2567953745524572</v>
       </c>
       <c r="L17">
@@ -31786,11 +31786,11 @@
         <v>17.800104133904998</v>
       </c>
       <c r="J18">
-        <f>H18/D18</f>
+        <f t="shared" si="2"/>
         <v>1.0704535664423642</v>
       </c>
       <c r="K18">
-        <f>I18/D18</f>
+        <f t="shared" si="3"/>
         <v>1.2714360095646426</v>
       </c>
       <c r="L18">
@@ -31827,11 +31827,11 @@
         <v>17.401801966883301</v>
       </c>
       <c r="J19">
-        <f>H19/D19</f>
+        <f t="shared" si="2"/>
         <v>1.0601561895564</v>
       </c>
       <c r="K19">
-        <f>I19/D19</f>
+        <f t="shared" si="3"/>
         <v>1.2429858547773787</v>
       </c>
       <c r="L19">
@@ -31868,11 +31868,11 @@
         <v>17.376908136478999</v>
       </c>
       <c r="J20">
-        <f>H20/D20</f>
+        <f t="shared" si="2"/>
         <v>1.0582474872022429</v>
       </c>
       <c r="K20">
-        <f>I20/D20</f>
+        <f t="shared" si="3"/>
         <v>1.2412077240342143</v>
       </c>
       <c r="L20">
@@ -31909,11 +31909,11 @@
         <v>17.3073212448469</v>
       </c>
       <c r="J21">
-        <f>H21/D21</f>
+        <f t="shared" si="2"/>
         <v>1.0515313772327144</v>
       </c>
       <c r="K21">
-        <f>I21/D21</f>
+        <f t="shared" si="3"/>
         <v>1.2362372317747785</v>
       </c>
       <c r="L21">
@@ -31989,11 +31989,11 @@
         <v>18.097080062698399</v>
       </c>
       <c r="J24">
-        <f>H24/D24</f>
+        <f t="shared" ref="J24:J32" si="4">H24/D24</f>
         <v>1.083609589118107</v>
       </c>
       <c r="K24">
-        <f>I24/D24</f>
+        <f t="shared" ref="K24:K32" si="5">I24/D24</f>
         <v>1.2926485759070285</v>
       </c>
       <c r="L24">
@@ -32030,11 +32030,11 @@
         <v>18.135865263970199</v>
       </c>
       <c r="J25">
-        <f>H25/D25</f>
+        <f t="shared" si="4"/>
         <v>1.0768591048234499</v>
       </c>
       <c r="K25">
-        <f>I25/D25</f>
+        <f t="shared" si="5"/>
         <v>1.2954189474264428</v>
       </c>
       <c r="L25">
@@ -32071,11 +32071,11 @@
         <v>17.330098343282099</v>
       </c>
       <c r="J26">
-        <f>H26/D26</f>
+        <f t="shared" si="4"/>
         <v>1.0649417391035356</v>
       </c>
       <c r="K26">
-        <f>I26/D26</f>
+        <f t="shared" si="5"/>
         <v>1.2378641673772928</v>
       </c>
       <c r="L26">
@@ -32112,11 +32112,11 @@
         <v>17.367830630017998</v>
       </c>
       <c r="J27">
-        <f>H27/D27</f>
+        <f t="shared" si="4"/>
         <v>1.0626569816259572</v>
       </c>
       <c r="K27">
-        <f>I27/D27</f>
+        <f t="shared" si="5"/>
         <v>1.2405593307155713</v>
       </c>
       <c r="L27">
@@ -32153,11 +32153,11 @@
         <v>17.503717898902501</v>
       </c>
       <c r="J28">
-        <f>H28/D28</f>
+        <f t="shared" si="4"/>
         <v>1.0641333665607715</v>
       </c>
       <c r="K28">
-        <f>I28/D28</f>
+        <f t="shared" si="5"/>
         <v>1.2502655642073215</v>
       </c>
       <c r="L28">
@@ -32194,11 +32194,11 @@
         <v>17.3264201453349</v>
       </c>
       <c r="J29">
-        <f>H29/D29</f>
+        <f t="shared" si="4"/>
         <v>1.0589107596816858</v>
       </c>
       <c r="K29">
-        <f>I29/D29</f>
+        <f t="shared" si="5"/>
         <v>1.237601438952493</v>
       </c>
       <c r="L29">
@@ -32235,11 +32235,11 @@
         <v>17.0559245738987</v>
       </c>
       <c r="J30">
-        <f>H30/D30</f>
+        <f t="shared" si="4"/>
         <v>1.0490366221772072</v>
       </c>
       <c r="K30">
-        <f>I30/D30</f>
+        <f t="shared" si="5"/>
         <v>1.2182803267070501</v>
       </c>
       <c r="L30">
@@ -32276,11 +32276,11 @@
         <v>17.026731381825002</v>
       </c>
       <c r="J31">
-        <f>H31/D31</f>
+        <f t="shared" si="4"/>
         <v>1.0470169099162498</v>
       </c>
       <c r="K31">
-        <f>I31/D31</f>
+        <f t="shared" si="5"/>
         <v>1.2161950987017858</v>
       </c>
       <c r="L31">
@@ -32317,11 +32317,11 @@
         <v>16.792322453345399</v>
       </c>
       <c r="J32">
-        <f>H32/D32</f>
+        <f t="shared" si="4"/>
         <v>1.0399532955002644</v>
       </c>
       <c r="K32">
-        <f>I32/D32</f>
+        <f t="shared" si="5"/>
         <v>1.1994516038103857</v>
       </c>
       <c r="L32">
@@ -32397,11 +32397,11 @@
         <v>18.089161596296702</v>
       </c>
       <c r="J35">
-        <f>H35/D35</f>
+        <f t="shared" ref="J35:J43" si="6">H35/D35</f>
         <v>1.0712144883827499</v>
       </c>
       <c r="K35">
-        <f>I35/D35</f>
+        <f t="shared" ref="K35:K43" si="7">I35/D35</f>
         <v>1.29208297116405</v>
       </c>
       <c r="L35">
@@ -32438,11 +32438,11 @@
         <v>17.570376223618901</v>
       </c>
       <c r="J36">
-        <f>H36/D36</f>
+        <f t="shared" si="6"/>
         <v>1.0596752495115787</v>
       </c>
       <c r="K36">
-        <f>I36/D36</f>
+        <f t="shared" si="7"/>
         <v>1.2550268731156358</v>
       </c>
       <c r="L36">
@@ -32479,11 +32479,11 @@
         <v>17.3536317422313</v>
       </c>
       <c r="J37">
-        <f>H37/D37</f>
+        <f t="shared" si="6"/>
         <v>1.0571856703432143</v>
       </c>
       <c r="K37">
-        <f>I37/D37</f>
+        <f t="shared" si="7"/>
         <v>1.2395451244450928</v>
       </c>
       <c r="L37">
@@ -32520,11 +32520,11 @@
         <v>17.291374788242202</v>
       </c>
       <c r="J38">
-        <f>H38/D38</f>
+        <f t="shared" si="6"/>
         <v>1.0519673938384857</v>
       </c>
       <c r="K38">
-        <f>I38/D38</f>
+        <f t="shared" si="7"/>
         <v>1.2350981991601573</v>
       </c>
       <c r="L38">
@@ -32561,11 +32561,11 @@
         <v>17.159997968615599</v>
       </c>
       <c r="J39">
-        <f>H39/D39</f>
+        <f t="shared" si="6"/>
         <v>1.0503864387710213</v>
       </c>
       <c r="K39">
-        <f>I39/D39</f>
+        <f t="shared" si="7"/>
         <v>1.2257141406154</v>
       </c>
       <c r="L39">
@@ -32602,11 +32602,11 @@
         <v>17.055866015880401</v>
       </c>
       <c r="J40">
-        <f>H40/D40</f>
+        <f t="shared" si="6"/>
         <v>1.0509062974190286</v>
       </c>
       <c r="K40">
-        <f>I40/D40</f>
+        <f t="shared" si="7"/>
         <v>1.2182761439914571</v>
       </c>
       <c r="L40">
@@ -32643,11 +32643,11 @@
         <v>16.980790413763099</v>
       </c>
       <c r="J41">
-        <f>H41/D41</f>
+        <f t="shared" si="6"/>
         <v>1.0448722017372072</v>
       </c>
       <c r="K41">
-        <f>I41/D41</f>
+        <f t="shared" si="7"/>
         <v>1.2129136009830785</v>
       </c>
       <c r="L41">
@@ -32684,11 +32684,11 @@
         <v>16.801664428376501</v>
       </c>
       <c r="J42">
-        <f>H42/D42</f>
+        <f t="shared" si="6"/>
         <v>1.039138043805657</v>
       </c>
       <c r="K42">
-        <f>I42/D42</f>
+        <f t="shared" si="7"/>
         <v>1.2001188877411786</v>
       </c>
       <c r="L42">
@@ -32725,11 +32725,11 @@
         <v>16.653992577441102</v>
       </c>
       <c r="J43">
-        <f>H43/D43</f>
+        <f t="shared" si="6"/>
         <v>1.0357093559246</v>
       </c>
       <c r="K43">
-        <f>I43/D43</f>
+        <f t="shared" si="7"/>
         <v>1.1895708983886502</v>
       </c>
       <c r="L43">
@@ -32805,11 +32805,11 @@
         <v>14.199385231429501</v>
       </c>
       <c r="J46">
-        <f>H46/D46</f>
+        <f t="shared" ref="J46:J54" si="8">H46/D46</f>
         <v>1.0014840555932285</v>
       </c>
       <c r="K46">
-        <f>I46/D46</f>
+        <f t="shared" ref="K46:K54" si="9">I46/D46</f>
         <v>1.0142418022449644</v>
       </c>
       <c r="L46">
@@ -32846,11 +32846,11 @@
         <v>14.5920185798697</v>
       </c>
       <c r="J47">
-        <f>H47/D47</f>
+        <f t="shared" si="8"/>
         <v>1.0048038624252</v>
       </c>
       <c r="K47">
-        <f>I47/D47</f>
+        <f t="shared" si="9"/>
         <v>1.0422870414192642</v>
       </c>
       <c r="L47">
@@ -32887,11 +32887,11 @@
         <v>14.709265508164799</v>
       </c>
       <c r="J48">
-        <f>H48/D48</f>
+        <f t="shared" si="8"/>
         <v>1.0063357941835787</v>
       </c>
       <c r="K48">
-        <f>I48/D48</f>
+        <f t="shared" si="9"/>
         <v>1.0506618220117714</v>
       </c>
       <c r="L48">
@@ -32928,11 +32928,11 @@
         <v>14.8641445687892</v>
       </c>
       <c r="J49">
-        <f>H49/D49</f>
+        <f t="shared" si="8"/>
         <v>1.00719126089855</v>
       </c>
       <c r="K49">
-        <f>I49/D49</f>
+        <f t="shared" si="9"/>
         <v>1.0617246120563715</v>
       </c>
       <c r="L49">
@@ -32969,11 +32969,11 @@
         <v>14.774248722916001</v>
       </c>
       <c r="J50">
-        <f>H50/D50</f>
+        <f t="shared" si="8"/>
         <v>1.0070782649004786</v>
       </c>
       <c r="K50">
-        <f>I50/D50</f>
+        <f t="shared" si="9"/>
         <v>1.0553034802082857</v>
       </c>
       <c r="L50">
@@ -33010,11 +33010,11 @@
         <v>14.7621191939502</v>
       </c>
       <c r="J51">
-        <f>H51/D51</f>
+        <f t="shared" si="8"/>
         <v>1.0075389934414571</v>
       </c>
       <c r="K51">
-        <f>I51/D51</f>
+        <f t="shared" si="9"/>
         <v>1.0544370852821572</v>
       </c>
       <c r="L51">
@@ -33051,11 +33051,11 @@
         <v>14.7934850986701</v>
       </c>
       <c r="J52">
-        <f>H52/D52</f>
+        <f t="shared" si="8"/>
         <v>1.0074755013547356</v>
       </c>
       <c r="K52">
-        <f>I52/D52</f>
+        <f t="shared" si="9"/>
         <v>1.0566775070478642</v>
       </c>
       <c r="L52">
@@ -33092,11 +33092,11 @@
         <v>14.835311382726299</v>
       </c>
       <c r="J53">
-        <f>H53/D53</f>
+        <f t="shared" si="8"/>
         <v>1.0078336907780072</v>
       </c>
       <c r="K53">
-        <f>I53/D53</f>
+        <f t="shared" si="9"/>
         <v>1.0596650987661642</v>
       </c>
       <c r="L53">
@@ -33133,11 +33133,11 @@
         <v>14.880267868774499</v>
       </c>
       <c r="J54">
-        <f>H54/D54</f>
+        <f t="shared" si="8"/>
         <v>1.0081929029355785</v>
       </c>
       <c r="K54">
-        <f>I54/D54</f>
+        <f t="shared" si="9"/>
         <v>1.0628762763410358</v>
       </c>
       <c r="L54">
@@ -33160,7 +33160,7 @@
   <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46:I54"/>
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33249,11 +33249,11 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <f>H2/D2</f>
+        <f t="shared" ref="J2:J10" si="0">H2/D2</f>
         <v>1</v>
       </c>
       <c r="K2">
-        <f>I2/D2</f>
+        <f t="shared" ref="K2:K10" si="1">I2/D2</f>
         <v>1</v>
       </c>
       <c r="L2">
@@ -33290,11 +33290,11 @@
         <v>14</v>
       </c>
       <c r="J3">
-        <f>H3/D3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K3">
-        <f>I3/D3</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L3">
@@ -33331,11 +33331,11 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <f>H4/D4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K4">
-        <f>I4/D4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L4">
@@ -33372,11 +33372,11 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <f>H5/D5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>I5/D5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L5">
@@ -33413,11 +33413,11 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <f>H6/D6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K6">
-        <f>I6/D6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L6">
@@ -33454,11 +33454,11 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <f>H7/D7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K7">
-        <f>I7/D7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L7">
@@ -33495,11 +33495,11 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <f>H8/D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f>I8/D8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L8">
@@ -33536,11 +33536,11 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <f>H9/D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f>I9/D9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L9">
@@ -33577,11 +33577,11 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <f>H10/D10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K10">
-        <f>I10/D10</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L10">
@@ -33657,11 +33657,11 @@
         <v>18.451275054955499</v>
       </c>
       <c r="J13">
-        <f>H13/D13</f>
+        <f t="shared" ref="J13:J21" si="2">H13/D13</f>
         <v>1.0832804049587073</v>
       </c>
       <c r="K13">
-        <f>I13/D13</f>
+        <f t="shared" ref="K13:K21" si="3">I13/D13</f>
         <v>1.3179482182111071</v>
       </c>
       <c r="L13">
@@ -33698,11 +33698,11 @@
         <v>18.010377669408399</v>
       </c>
       <c r="J14">
-        <f>H14/D14</f>
+        <f t="shared" si="2"/>
         <v>1.0732831226056714</v>
       </c>
       <c r="K14">
-        <f>I14/D14</f>
+        <f t="shared" si="3"/>
         <v>1.2864555478148856</v>
       </c>
       <c r="L14">
@@ -33739,11 +33739,11 @@
         <v>17.552972338711299</v>
       </c>
       <c r="J15">
-        <f>H15/D15</f>
+        <f t="shared" si="2"/>
         <v>1.0654568414356285</v>
       </c>
       <c r="K15">
-        <f>I15/D15</f>
+        <f t="shared" si="3"/>
         <v>1.2537837384793786</v>
       </c>
       <c r="L15">
@@ -33780,11 +33780,11 @@
         <v>17.4517792054437</v>
       </c>
       <c r="J16">
-        <f>H16/D16</f>
+        <f t="shared" si="2"/>
         <v>1.0631957660006714</v>
       </c>
       <c r="K16">
-        <f>I16/D16</f>
+        <f t="shared" si="3"/>
         <v>1.2465556575316927</v>
       </c>
       <c r="L16">
@@ -33821,11 +33821,11 @@
         <v>17.181026463842699</v>
       </c>
       <c r="J17">
-        <f>H17/D17</f>
+        <f t="shared" si="2"/>
         <v>1.057786380910843</v>
       </c>
       <c r="K17">
-        <f>I17/D17</f>
+        <f t="shared" si="3"/>
         <v>1.2272161759887641</v>
       </c>
       <c r="L17">
@@ -33862,11 +33862,11 @@
         <v>17.274140984923399</v>
       </c>
       <c r="J18">
-        <f>H18/D18</f>
+        <f t="shared" si="2"/>
         <v>1.0609048618286498</v>
       </c>
       <c r="K18">
-        <f>I18/D18</f>
+        <f t="shared" si="3"/>
         <v>1.2338672132088142</v>
       </c>
       <c r="L18">
@@ -33903,11 +33903,11 @@
         <v>17.004476815393598</v>
       </c>
       <c r="J19">
-        <f>H19/D19</f>
+        <f t="shared" si="2"/>
         <v>1.0530825595218642</v>
       </c>
       <c r="K19">
-        <f>I19/D19</f>
+        <f t="shared" si="3"/>
         <v>1.2146054868138285</v>
       </c>
       <c r="L19">
@@ -33944,11 +33944,11 @@
         <v>16.970682682277701</v>
       </c>
       <c r="J20">
-        <f>H20/D20</f>
+        <f t="shared" si="2"/>
         <v>1.0510927495952642</v>
       </c>
       <c r="K20">
-        <f>I20/D20</f>
+        <f t="shared" si="3"/>
         <v>1.212191620162693</v>
       </c>
       <c r="L20">
@@ -33985,11 +33985,11 @@
         <v>16.766722797469999</v>
       </c>
       <c r="J21">
-        <f>H21/D21</f>
+        <f t="shared" si="2"/>
         <v>1.0438890278196928</v>
       </c>
       <c r="K21">
-        <f>I21/D21</f>
+        <f t="shared" si="3"/>
         <v>1.1976230569621429</v>
       </c>
       <c r="L21">
@@ -34065,11 +34065,11 @@
         <v>17.462681181174201</v>
       </c>
       <c r="J24">
-        <f>H24/D24</f>
+        <f t="shared" ref="J24:J32" si="4">H24/D24</f>
         <v>1.0715893766619571</v>
       </c>
       <c r="K24">
-        <f>I24/D24</f>
+        <f t="shared" ref="K24:K32" si="5">I24/D24</f>
         <v>1.2473343700838715</v>
       </c>
       <c r="L24">
@@ -34106,11 +34106,11 @@
         <v>17.438312038237601</v>
       </c>
       <c r="J25">
-        <f>H25/D25</f>
+        <f t="shared" si="4"/>
         <v>1.0654696498407643</v>
       </c>
       <c r="K25">
-        <f>I25/D25</f>
+        <f t="shared" si="5"/>
         <v>1.2455937170169715</v>
       </c>
       <c r="L25">
@@ -34147,11 +34147,11 @@
         <v>17.0028941055443</v>
       </c>
       <c r="J26">
-        <f>H26/D26</f>
+        <f t="shared" si="4"/>
         <v>1.0566653946553142</v>
       </c>
       <c r="K26">
-        <f>I26/D26</f>
+        <f t="shared" si="5"/>
         <v>1.2144924361103071</v>
       </c>
       <c r="L26">
@@ -34188,11 +34188,11 @@
         <v>16.994741019407599</v>
       </c>
       <c r="J27">
-        <f>H27/D27</f>
+        <f t="shared" si="4"/>
         <v>1.0541556507774357</v>
       </c>
       <c r="K27">
-        <f>I27/D27</f>
+        <f t="shared" si="5"/>
         <v>1.2139100728148284</v>
       </c>
       <c r="L27">
@@ -34229,11 +34229,11 @@
         <v>17.004243344147799</v>
       </c>
       <c r="J28">
-        <f>H28/D28</f>
+        <f t="shared" si="4"/>
         <v>1.0549982974981214</v>
       </c>
       <c r="K28">
-        <f>I28/D28</f>
+        <f t="shared" si="5"/>
         <v>1.2145888102962714</v>
       </c>
       <c r="L28">
@@ -34270,11 +34270,11 @@
         <v>16.938695345471199</v>
       </c>
       <c r="J29">
-        <f>H29/D29</f>
+        <f t="shared" si="4"/>
         <v>1.0529895625360142</v>
       </c>
       <c r="K29">
-        <f>I29/D29</f>
+        <f t="shared" si="5"/>
         <v>1.2099068103907999</v>
       </c>
       <c r="L29">
@@ -34311,11 +34311,11 @@
         <v>16.7086846647206</v>
       </c>
       <c r="J30">
-        <f>H30/D30</f>
+        <f t="shared" si="4"/>
         <v>1.0442064049061215</v>
       </c>
       <c r="K30">
-        <f>I30/D30</f>
+        <f t="shared" si="5"/>
         <v>1.1934774760514715</v>
       </c>
       <c r="L30">
@@ -34352,11 +34352,11 @@
         <v>16.683560813910798</v>
       </c>
       <c r="J31">
-        <f>H31/D31</f>
+        <f t="shared" si="4"/>
         <v>1.0424580441499858</v>
       </c>
       <c r="K31">
-        <f>I31/D31</f>
+        <f t="shared" si="5"/>
         <v>1.1916829152793427</v>
       </c>
       <c r="L31">
@@ -34393,11 +34393,11 @@
         <v>16.450925167062898</v>
       </c>
       <c r="J32">
-        <f>H32/D32</f>
+        <f t="shared" si="4"/>
         <v>1.0357629852363215</v>
       </c>
       <c r="K32">
-        <f>I32/D32</f>
+        <f t="shared" si="5"/>
         <v>1.1750660833616355</v>
       </c>
       <c r="L32">
@@ -34473,11 +34473,11 @@
         <v>17.8714428251626</v>
       </c>
       <c r="J35">
-        <f>H35/D35</f>
+        <f t="shared" ref="J35:J43" si="6">H35/D35</f>
         <v>1.0644856188692786</v>
       </c>
       <c r="K35">
-        <f>I35/D35</f>
+        <f t="shared" ref="K35:K43" si="7">I35/D35</f>
         <v>1.2765316303687571</v>
       </c>
       <c r="L35">
@@ -34514,11 +34514,11 @@
         <v>17.1333557705115</v>
       </c>
       <c r="J36">
-        <f>H36/D36</f>
+        <f t="shared" si="6"/>
         <v>1.0516058853163928</v>
       </c>
       <c r="K36">
-        <f>I36/D36</f>
+        <f t="shared" si="7"/>
         <v>1.223811126465107</v>
       </c>
       <c r="L36">
@@ -34555,11 +34555,11 @@
         <v>16.846707459819601</v>
       </c>
       <c r="J37">
-        <f>H37/D37</f>
+        <f t="shared" si="6"/>
         <v>1.0484613526016</v>
       </c>
       <c r="K37">
-        <f>I37/D37</f>
+        <f t="shared" si="7"/>
         <v>1.2033362471299716</v>
       </c>
       <c r="L37">
@@ -34596,11 +34596,11 @@
         <v>16.824269943278999</v>
       </c>
       <c r="J38">
-        <f>H38/D38</f>
+        <f t="shared" si="6"/>
         <v>1.0443862422568786</v>
       </c>
       <c r="K38">
-        <f>I38/D38</f>
+        <f t="shared" si="7"/>
         <v>1.2017335673770713</v>
       </c>
       <c r="L38">
@@ -34637,11 +34637,11 @@
         <v>16.6940399724336</v>
       </c>
       <c r="J39">
-        <f>H39/D39</f>
+        <f t="shared" si="6"/>
         <v>1.0434110949927928</v>
       </c>
       <c r="K39">
-        <f>I39/D39</f>
+        <f t="shared" si="7"/>
         <v>1.1924314266024001</v>
       </c>
       <c r="L39">
@@ -34678,11 +34678,11 @@
         <v>16.720104777918898</v>
       </c>
       <c r="J40">
-        <f>H40/D40</f>
+        <f t="shared" si="6"/>
         <v>1.0446635343914499</v>
       </c>
       <c r="K40">
-        <f>I40/D40</f>
+        <f t="shared" si="7"/>
         <v>1.1942931984227785</v>
       </c>
       <c r="L40">
@@ -34719,11 +34719,11 @@
         <v>16.502857196436601</v>
       </c>
       <c r="J41">
-        <f>H41/D41</f>
+        <f t="shared" si="6"/>
         <v>1.0378818389295998</v>
       </c>
       <c r="K41">
-        <f>I41/D41</f>
+        <f t="shared" si="7"/>
         <v>1.1787755140311857</v>
       </c>
       <c r="L41">
@@ -34760,11 +34760,11 @@
         <v>16.449860394696199</v>
       </c>
       <c r="J42">
-        <f>H42/D42</f>
+        <f t="shared" si="6"/>
         <v>1.03376506502065</v>
       </c>
       <c r="K42">
-        <f>I42/D42</f>
+        <f t="shared" si="7"/>
         <v>1.1749900281925856</v>
       </c>
       <c r="L42">
@@ -34801,11 +34801,11 @@
         <v>16.268893357120898</v>
       </c>
       <c r="J43">
-        <f>H43/D43</f>
+        <f t="shared" si="6"/>
         <v>1.0298840910925571</v>
       </c>
       <c r="K43">
-        <f>I43/D43</f>
+        <f t="shared" si="7"/>
         <v>1.1620638112229214</v>
       </c>
       <c r="L43">
@@ -34881,11 +34881,11 @@
         <v>14.182714015677799</v>
       </c>
       <c r="J46">
-        <f>H46/D46</f>
+        <f t="shared" ref="J46:J54" si="8">H46/D46</f>
         <v>1.0013569574973071</v>
       </c>
       <c r="K46">
-        <f>I46/D46</f>
+        <f t="shared" ref="K46:K54" si="9">I46/D46</f>
         <v>1.0130510011198428</v>
       </c>
       <c r="L46">
@@ -34922,11 +34922,11 @@
         <v>14.521396600901801</v>
       </c>
       <c r="J47">
-        <f>H47/D47</f>
+        <f t="shared" si="8"/>
         <v>1.0041757584049642</v>
       </c>
       <c r="K47">
-        <f>I47/D47</f>
+        <f t="shared" si="9"/>
         <v>1.0372426143501285</v>
       </c>
       <c r="L47">
@@ -34963,11 +34963,11 @@
         <v>14.6141138263807</v>
       </c>
       <c r="J48">
-        <f>H48/D48</f>
+        <f t="shared" si="8"/>
         <v>1.0053775059363215</v>
       </c>
       <c r="K48">
-        <f>I48/D48</f>
+        <f t="shared" si="9"/>
         <v>1.0438652733129072</v>
       </c>
       <c r="L48">
@@ -35004,11 +35004,11 @@
         <v>14.7080736321915</v>
       </c>
       <c r="J49">
-        <f>H49/D49</f>
+        <f t="shared" si="8"/>
         <v>1.0059299093087428</v>
       </c>
       <c r="K49">
-        <f>I49/D49</f>
+        <f t="shared" si="9"/>
         <v>1.0505766880136787</v>
       </c>
       <c r="L49">
@@ -35045,11 +35045,11 @@
         <v>14.6863697612901</v>
       </c>
       <c r="J50">
-        <f>H50/D50</f>
+        <f t="shared" si="8"/>
         <v>1.0062969574230716</v>
       </c>
       <c r="K50">
-        <f>I50/D50</f>
+        <f t="shared" si="9"/>
         <v>1.0490264115207215</v>
       </c>
       <c r="L50">
@@ -35086,11 +35086,11 @@
         <v>14.6753778211918</v>
       </c>
       <c r="J51">
-        <f>H51/D51</f>
+        <f t="shared" si="8"/>
         <v>1.0065765709454857</v>
       </c>
       <c r="K51">
-        <f>I51/D51</f>
+        <f t="shared" si="9"/>
         <v>1.0482412729422714</v>
       </c>
       <c r="L51">
@@ -35127,11 +35127,11 @@
         <v>14.675412682483101</v>
       </c>
       <c r="J52">
-        <f>H52/D52</f>
+        <f t="shared" si="8"/>
         <v>1.0063980246537929</v>
       </c>
       <c r="K52">
-        <f>I52/D52</f>
+        <f t="shared" si="9"/>
         <v>1.0482437630345072</v>
       </c>
       <c r="L52">
@@ -35168,11 +35168,11 @@
         <v>14.7317643159829</v>
       </c>
       <c r="J53">
-        <f>H53/D53</f>
+        <f t="shared" si="8"/>
         <v>1.0069882275144</v>
       </c>
       <c r="K53">
-        <f>I53/D53</f>
+        <f t="shared" si="9"/>
         <v>1.0522688797130644</v>
       </c>
       <c r="L53">
@@ -35209,11 +35209,11 @@
         <v>14.800076012225601</v>
       </c>
       <c r="J54">
-        <f>H54/D54</f>
+        <f t="shared" si="8"/>
         <v>1.0077349850813428</v>
       </c>
       <c r="K54">
-        <f>I54/D54</f>
+        <f t="shared" si="9"/>
         <v>1.057148286587543</v>
       </c>
       <c r="L54">

</xml_diff>